<commit_message>
Add extracting foods and meals to excel functionality
</commit_message>
<xml_diff>
--- a/foods_log.xlsx
+++ b/foods_log.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -500,10 +500,10 @@
         <v>64</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>17.3</v>
+        <v>17</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -535,19 +535,19 @@
         <v>97</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>22.7</v>
+        <v>23</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0.18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -576,7 +576,7 @@
         <v>69</v>
       </c>
       <c r="G4" t="n">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="H4" t="n">
         <v>8</v>
@@ -611,24 +611,24 @@
         <v>11</v>
       </c>
       <c r="G5" t="n">
-        <v>8.5</v>
+        <v>9</v>
       </c>
       <c r="H5" t="n">
         <v>58</v>
       </c>
       <c r="I5" t="n">
-        <v>0.55</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Yogurt</t>
+          <t>Protein_Pudding</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Fage</t>
+          <t>Alpro</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -637,63 +637,63 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E6" t="n">
-        <v>19.9</v>
+        <v>10</v>
       </c>
       <c r="F6" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G6" t="n">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="H6" t="n">
         <v>2</v>
       </c>
       <c r="I6" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Protein_Pudding</t>
+          <t>Egg</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Alpro</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>100g</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F7" t="n">
-        <v>6.6</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.9</v>
+        <v>2</v>
       </c>
       <c r="H7" t="n">
-        <v>1.5</v>
+        <v>5</v>
       </c>
       <c r="I7" t="n">
-        <v>0.19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Egg</t>
+          <t>Cucumber</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -703,102 +703,102 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1(medium)</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>72</v>
+        <v>30</v>
       </c>
       <c r="E8" t="n">
-        <v>6.3</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>0.4</v>
+        <v>7</v>
       </c>
       <c r="G8" t="n">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>4.8</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>0.71</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Cucumber</t>
+          <t>GroundBeaf</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Coocked(lean)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1(medium)</t>
+          <t>100g</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>30</v>
+        <v>270</v>
       </c>
       <c r="E9" t="n">
-        <v>1.3</v>
+        <v>27</v>
       </c>
       <c r="F9" t="n">
-        <v>7.3</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="I9" t="n">
-        <v>0.04</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>GroundBeaf</t>
+          <t>Banana</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Coocked(lean)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>100g</t>
+          <t>1(medium)</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>270</v>
+        <v>105</v>
       </c>
       <c r="E10" t="n">
-        <v>27.1</v>
+        <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="G10" t="n">
-        <v>6.5</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>17.5</v>
+        <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>0.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Banana</t>
+          <t>Egg_white</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -808,67 +808,67 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>1(medium)</t>
+          <t>1(from 1 egg)</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>105</v>
+        <v>17</v>
       </c>
       <c r="E11" t="n">
-        <v>1.3</v>
+        <v>4</v>
       </c>
       <c r="F11" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>0.12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Egg_white</t>
+          <t>Rasberries</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Frozen</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1(from 1 egg)</t>
+          <t>100g</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="E12" t="n">
-        <v>3.6</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>0.2</v>
+        <v>5</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>0.55</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Rasberries</t>
+          <t>Strawberries</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -882,115 +882,115 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E13" t="n">
-        <v>1.4</v>
+        <v>1</v>
       </c>
       <c r="F13" t="n">
-        <v>4.6</v>
+        <v>7</v>
       </c>
       <c r="G13" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Strawberries</t>
+          <t>Bread</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Frozen</t>
+          <t>Brown</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>100g</t>
+          <t>1(slice)</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="E14" t="n">
-        <v>0.8</v>
+        <v>2</v>
       </c>
       <c r="F14" t="n">
-        <v>7.4</v>
+        <v>11</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="I14" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Bread</t>
+          <t>Chichen</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Brown</t>
+          <t>Breast</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>1(slice)</t>
+          <t>100g</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>61</v>
+        <v>169</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="F15" t="n">
-        <v>10.8</v>
+        <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="H15" t="n">
-        <v>0.9</v>
+        <v>4</v>
       </c>
       <c r="I15" t="n">
-        <v>0.27</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Chichen</t>
+          <t>OliveOil</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Breast</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>100g</t>
+          <t>1 tablespoon</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>169</v>
+        <v>83</v>
       </c>
       <c r="E16" t="n">
-        <v>31.5</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -999,42 +999,42 @@
         <v>1</v>
       </c>
       <c r="H16" t="n">
-        <v>3.7</v>
+        <v>10</v>
       </c>
       <c r="I16" t="n">
-        <v>0.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>OliveOil</t>
+          <t>Tomato</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Cherry</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1 tablespoon</t>
+          <t>100g</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>83.3</v>
+        <v>18</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G17" t="n">
-        <v>1.3</v>
+        <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>9.800000000000001</v>
+        <v>0</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
@@ -1043,12 +1043,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Tomato</t>
+          <t>Spinach</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Cherry</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1057,33 +1057,33 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>17.6</v>
+        <v>23</v>
       </c>
       <c r="E18" t="n">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>3.8</v>
+        <v>3</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>0.05</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Spinach</t>
+          <t>BabyPotatos</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AB</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1092,28 +1092,28 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>22.7</v>
+        <v>77</v>
       </c>
       <c r="E19" t="n">
-        <v>0.28</v>
+        <v>2</v>
       </c>
       <c r="F19" t="n">
-        <v>3.3</v>
+        <v>17</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>BabyPotatos</t>
+          <t>Fakes</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1127,28 +1127,28 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>77</v>
+        <v>329</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="F20" t="n">
-        <v>17.46</v>
+        <v>48</v>
       </c>
       <c r="G20" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="I20" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Fakes</t>
+          <t>Paksimadi(Krithino)</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1162,243 +1162,243 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>329</v>
+        <v>376</v>
       </c>
       <c r="E21" t="n">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F21" t="n">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="G21" t="n">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="H21" t="n">
-        <v>1.3</v>
+        <v>4</v>
       </c>
       <c r="I21" t="n">
-        <v>0.03</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Paksimadi(Krithino)</t>
+          <t>AlmondMilk</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>AB</t>
+          <t>Delta</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>100g</t>
+          <t>100ml</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>376</v>
+        <v>31</v>
       </c>
       <c r="E22" t="n">
-        <v>11.2</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
-        <v>68.40000000000001</v>
+        <v>3</v>
       </c>
       <c r="G22" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="H22" t="n">
-        <v>3.8</v>
+        <v>2</v>
       </c>
       <c r="I22" t="n">
-        <v>2.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>AlmondMilk</t>
+          <t>Salad</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Delta</t>
+          <t>AB</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>100ml</t>
+          <t>100g</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>31</v>
+        <v>103</v>
       </c>
       <c r="E23" t="n">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H23" t="n">
-        <v>1.7</v>
+        <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Salad</t>
+          <t>Scoop</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>AB</t>
+          <t>Biotech</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>100g</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F24" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" t="n">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="I24" t="n">
-        <v>0.07000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Scoop</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Biotech</t>
+          <t>Basmati</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>100g</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>120</v>
+        <v>351</v>
       </c>
       <c r="E25" t="n">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F25" t="n">
-        <v>1.8</v>
+        <v>76</v>
       </c>
       <c r="G25" t="n">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="H25" t="n">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="I25" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Rice</t>
+          <t>Mustard</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Basmati</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>100g</t>
+          <t>1tpsp</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>351</v>
+        <v>10</v>
       </c>
       <c r="E26" t="n">
-        <v>7.5</v>
+        <v>1</v>
       </c>
       <c r="F26" t="n">
-        <v>76.40000000000001</v>
+        <v>1</v>
       </c>
       <c r="G26" t="n">
-        <v>1.4</v>
+        <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="I26" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Mustard</t>
+          <t>Yogurt_sauce</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Plain</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>1tpsp</t>
+          <t>100g</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="E27" t="n">
-        <v>0.6</v>
+        <v>19</v>
       </c>
       <c r="F27" t="n">
-        <v>0.9</v>
+        <v>4</v>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H27" t="n">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="I27" t="n">
-        <v>0.16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Yogurt_sauce</t>
+          <t>Beef_stake</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Plain</t>
+          <t>Lean</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1407,33 +1407,33 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>73</v>
+        <v>250</v>
       </c>
       <c r="E28" t="n">
-        <v>18.8</v>
+        <v>27</v>
       </c>
       <c r="F28" t="n">
-        <v>3.6</v>
+        <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>2.2</v>
+        <v>5</v>
       </c>
       <c r="H28" t="n">
-        <v>1.17</v>
+        <v>15</v>
       </c>
       <c r="I28" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Beef_stake</t>
+          <t>Corn_boiled</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Lean</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1442,28 +1442,28 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>250</v>
+        <v>108</v>
       </c>
       <c r="E29" t="n">
-        <v>27.2</v>
+        <v>3</v>
       </c>
       <c r="F29" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G29" t="n">
-        <v>5.2</v>
+        <v>0</v>
       </c>
       <c r="H29" t="n">
-        <v>15.2</v>
+        <v>1</v>
       </c>
       <c r="I29" t="n">
-        <v>0.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Corn_boiled</t>
+          <t>Tsipoura</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1473,32 +1473,32 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>100g</t>
+          <t>100</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>108</v>
+        <v>144</v>
       </c>
       <c r="E30" t="n">
-        <v>3.32</v>
+        <v>20</v>
       </c>
       <c r="F30" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>0.1</v>
+        <v>3</v>
       </c>
       <c r="H30" t="n">
-        <v>1.18</v>
+        <v>7</v>
       </c>
       <c r="I30" t="n">
-        <v>0.017</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Tsipoura</t>
+          <t>Feta_Cheese</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1508,32 +1508,32 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>100g</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>144</v>
+        <v>270</v>
       </c>
       <c r="E31" t="n">
-        <v>20.3</v>
+        <v>14</v>
       </c>
       <c r="F31" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G31" t="n">
-        <v>2.5</v>
+        <v>15</v>
       </c>
       <c r="H31" t="n">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="I31" t="n">
-        <v>0.23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Feta_Cheese</t>
+          <t>Olives</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1543,72 +1543,72 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>100g</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>270</v>
+        <v>3</v>
       </c>
       <c r="E32" t="n">
-        <v>14.4</v>
+        <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>4.3</v>
+        <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>15.1</v>
+        <v>0</v>
       </c>
       <c r="H32" t="n">
-        <v>26.1</v>
+        <v>0</v>
       </c>
       <c r="I32" t="n">
-        <v>0.93</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Olives</t>
+          <t>Penes</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AB</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>100g</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>3.3</v>
+        <v>343</v>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F33" t="n">
-        <v>0.2</v>
+        <v>65</v>
       </c>
       <c r="G33" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="H33" t="n">
-        <v>0.1</v>
+        <v>3</v>
       </c>
       <c r="I33" t="n">
-        <v>0.028</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Penes</t>
+          <t>Pita</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>AB</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1617,33 +1617,33 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>343</v>
+        <v>250</v>
       </c>
       <c r="E34" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F34" t="n">
-        <v>64.5</v>
+        <v>50</v>
       </c>
       <c r="G34" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="I34" t="n">
-        <v>0.06</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Pita</t>
+          <t>Cheese</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Dirollo</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1652,33 +1652,33 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>250</v>
+        <v>272</v>
       </c>
       <c r="E35" t="n">
-        <v>8.300000000000001</v>
+        <v>32</v>
       </c>
       <c r="F35" t="n">
-        <v>49.5</v>
+        <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>0.2</v>
+        <v>11</v>
       </c>
       <c r="H35" t="n">
-        <v>1.1</v>
+        <v>16</v>
       </c>
       <c r="I35" t="n">
-        <v>0.02</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Cheese</t>
+          <t>Tuna(water)</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Dirollo</t>
+          <t>AB</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1687,19 +1687,19 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>272</v>
+        <v>100</v>
       </c>
       <c r="E36" t="n">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F36" t="n">
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="H36" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="I36" t="n">
         <v>1</v>
@@ -1708,71 +1708,596 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Tuna(water)</t>
+          <t>Tortilla</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>AB</t>
+          <t>HighProtein</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>100g</t>
+          <t>1(62.5g)</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>100</v>
+        <v>197</v>
       </c>
       <c r="E37" t="n">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F37" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="G37" t="n">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="H37" t="n">
-        <v>0.9</v>
+        <v>4</v>
       </c>
       <c r="I37" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Tortilla</t>
+          <t>Yogurt</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>HighProtein</t>
+          <t>Olympos</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>1(62.5g)</t>
+          <t>100g</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>197</v>
+        <v>72</v>
       </c>
       <c r="E38" t="n">
-        <v>11.2</v>
+        <v>10</v>
       </c>
       <c r="F38" t="n">
-        <v>27.1</v>
+        <v>4</v>
       </c>
       <c r="G38" t="n">
-        <v>1.8</v>
+        <v>1</v>
       </c>
       <c r="H38" t="n">
-        <v>4.1</v>
+        <v>2</v>
       </c>
       <c r="I38" t="n">
-        <v>0.9399999999999999</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Ground beef</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Cooked(80-20)</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>100g</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>246</v>
+      </c>
+      <c r="E39" t="n">
+        <v>24</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>6</v>
+      </c>
+      <c r="H39" t="n">
+        <v>16</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Protein Powder</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Dymatize iso 100</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>1 scoop (32g)</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>120</v>
+      </c>
+      <c r="E40" t="n">
+        <v>25</v>
+      </c>
+      <c r="F40" t="n">
+        <v>2</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" t="n">
+        <v>1</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Granola</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Healthy Habits</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>100g</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>478</v>
+      </c>
+      <c r="E41" t="n">
+        <v>10</v>
+      </c>
+      <c r="F41" t="n">
+        <v>56</v>
+      </c>
+      <c r="G41" t="n">
+        <v>4</v>
+      </c>
+      <c r="H41" t="n">
+        <v>21</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Almond Milk</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Olympos</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>100ml</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>24</v>
+      </c>
+      <c r="E42" t="n">
+        <v>1</v>
+      </c>
+      <c r="F42" t="n">
+        <v>1</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Egg whites</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Xrysa Avga</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>100g</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>46</v>
+      </c>
+      <c r="E43" t="n">
+        <v>11</v>
+      </c>
+      <c r="F43" t="n">
+        <v>1</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Rice</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Basmati (Indian)</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>100g</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>358</v>
+      </c>
+      <c r="E44" t="n">
+        <v>8</v>
+      </c>
+      <c r="F44" t="n">
+        <v>78</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" t="n">
+        <v>1</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Cashews</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>EMMA</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>100g</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>627</v>
+      </c>
+      <c r="E45" t="n">
+        <v>17</v>
+      </c>
+      <c r="F45" t="n">
+        <v>30</v>
+      </c>
+      <c r="G45" t="n">
+        <v>9</v>
+      </c>
+      <c r="H45" t="n">
+        <v>48</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Walnuts</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>EMMA</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>100g</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>708</v>
+      </c>
+      <c r="E46" t="n">
+        <v>17</v>
+      </c>
+      <c r="F46" t="n">
+        <v>5</v>
+      </c>
+      <c r="G46" t="n">
+        <v>7</v>
+      </c>
+      <c r="H46" t="n">
+        <v>68</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Forest Fruits</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Gustona</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>100g</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>43</v>
+      </c>
+      <c r="E47" t="n">
+        <v>1</v>
+      </c>
+      <c r="F47" t="n">
+        <v>5</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>PeanutButter</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Haitoglou</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>100g</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>610</v>
+      </c>
+      <c r="E48" t="n">
+        <v>22</v>
+      </c>
+      <c r="F48" t="n">
+        <v>17</v>
+      </c>
+      <c r="G48" t="n">
+        <v>9</v>
+      </c>
+      <c r="H48" t="n">
+        <v>49</v>
+      </c>
+      <c r="I48" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Dates</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>EMMA</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>100g</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>469</v>
+      </c>
+      <c r="E49" t="n">
+        <v>2</v>
+      </c>
+      <c r="F49" t="n">
+        <v>75</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Straberry Jam</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Health Habits</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>100g</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>244</v>
+      </c>
+      <c r="E50" t="n">
+        <v>1</v>
+      </c>
+      <c r="F50" t="n">
+        <v>60</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>yogurt</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Fage</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>100g</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>70</v>
+      </c>
+      <c r="E51" t="n">
+        <v>10</v>
+      </c>
+      <c r="F51" t="n">
+        <v>3</v>
+      </c>
+      <c r="G51" t="n">
+        <v>1</v>
+      </c>
+      <c r="H51" t="n">
+        <v>2</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Pita Kalampokiou</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Karamolegos</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>1(82g)</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>217</v>
+      </c>
+      <c r="E52" t="n">
+        <v>6</v>
+      </c>
+      <c r="F52" t="n">
+        <v>43</v>
+      </c>
+      <c r="G52" t="n">
+        <v>1</v>
+      </c>
+      <c r="H52" t="n">
+        <v>2</v>
+      </c>
+      <c r="I52" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Turkey Patties</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Power in Meat</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>100g</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>145</v>
+      </c>
+      <c r="E53" t="n">
+        <v>29</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0</v>
+      </c>
+      <c r="H53" t="n">
+        <v>1</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Major fitness app improvements: user management, PDF export, meal macros, bug fixes
- Add comprehensive user management (create/edit/delete users)
- Implement PDF export for weekly meal plans with charts
- Add real-time macro calculator to Create Meal tab
- Fix nested parentheses parsing bug for foods like 'Ground beef (Cooked(80-20))'
- Add delete functionality for unassigned daily plans
- Improve meal/food selection with detailed labels and measurements
- Add goal-based TDEE display in daily planner
- Enhance weekly plan builder with user-centric approach
- Fix meal management IndexError and AttributeError issues
- Add debug tools for food lookup troubleshooting
- Update database schema with new user goal fields
</commit_message>
<xml_diff>
--- a/foods_log.xlsx
+++ b/foods_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -973,33 +973,33 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>OliveOil</t>
+          <t>Tomato</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Cherry</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>1 tablespoon</t>
+          <t>100g</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>83</v>
+        <v>18</v>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
@@ -1008,12 +1008,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Tomato</t>
+          <t>Spinach</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Cherry</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1022,13 +1022,13 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
@@ -1037,18 +1037,18 @@
         <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Spinach</t>
+          <t>BabyPotatos</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AB</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1057,13 +1057,13 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F18" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
@@ -1072,13 +1072,13 @@
         <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>BabyPotatos</t>
+          <t>Fakes</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1092,19 +1092,19 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>77</v>
+        <v>329</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="F19" t="n">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" t="n">
         <v>0</v>
@@ -1113,7 +1113,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Fakes</t>
+          <t>Paksimadi(Krithino)</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1127,89 +1127,89 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>329</v>
+        <v>376</v>
       </c>
       <c r="E20" t="n">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F20" t="n">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Paksimadi(Krithino)</t>
+          <t>AlmondMilk</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>AB</t>
+          <t>Delta</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>100g</t>
+          <t>100ml</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>376</v>
+        <v>31</v>
       </c>
       <c r="E21" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F21" t="n">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="G21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I21" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>AlmondMilk</t>
+          <t>Salad</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Delta</t>
+          <t>AB</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>100ml</t>
+          <t>100g</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>31</v>
+        <v>103</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G22" t="n">
         <v>0</v>
       </c>
       <c r="H22" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I22" t="n">
         <v>0</v>
@@ -1218,33 +1218,33 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Salad</t>
+          <t>Scoop</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>AB</t>
+          <t>Biotech</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>100g</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I23" t="n">
         <v>0</v>
@@ -1253,33 +1253,33 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Scoop</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Biotech</t>
+          <t>Basmati</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>100g</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>120</v>
+        <v>351</v>
       </c>
       <c r="E24" t="n">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
-        <v>2</v>
+        <v>76</v>
       </c>
       <c r="G24" t="n">
         <v>1</v>
       </c>
       <c r="H24" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I24" t="n">
         <v>0</v>
@@ -1288,30 +1288,30 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Rice</t>
+          <t>Mustard</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Basmati</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>100g</t>
+          <t>1tpsp</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>351</v>
+        <v>10</v>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="G25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
@@ -1323,33 +1323,33 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Mustard</t>
+          <t>Yogurt_sauce</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Plain</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>1tpsp</t>
+          <t>100g</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="F26" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G26" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" t="n">
         <v>0</v>
@@ -1358,12 +1358,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Yogurt_sauce</t>
+          <t>Beef_stake</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Plain</t>
+          <t>Lean</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1372,19 +1372,19 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>73</v>
+        <v>250</v>
       </c>
       <c r="E27" t="n">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F27" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H27" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="I27" t="n">
         <v>0</v>
@@ -1393,12 +1393,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Beef_stake</t>
+          <t>Corn_boiled</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Lean</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1407,19 +1407,19 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>250</v>
+        <v>108</v>
       </c>
       <c r="E28" t="n">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="F28" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G28" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H28" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
@@ -1428,7 +1428,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Corn_boiled</t>
+          <t>Tsipoura</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1438,23 +1438,23 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>100g</t>
+          <t>100</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>108</v>
+        <v>144</v>
       </c>
       <c r="E29" t="n">
+        <v>20</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="n">
         <v>3</v>
       </c>
-      <c r="F29" t="n">
-        <v>25</v>
-      </c>
-      <c r="G29" t="n">
-        <v>0</v>
-      </c>
       <c r="H29" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I29" t="n">
         <v>0</v>
@@ -1463,7 +1463,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Tsipoura</t>
+          <t>Feta_Cheese</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1473,32 +1473,32 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>100g</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>144</v>
+        <v>270</v>
       </c>
       <c r="E30" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F30" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G30" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="H30" t="n">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Feta_Cheese</t>
+          <t>Olives</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1508,58 +1508,58 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>100g</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>270</v>
+        <v>3</v>
       </c>
       <c r="E31" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H31" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="I31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Olives</t>
+          <t>Penes</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AB</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>100g</t>
         </is>
       </c>
       <c r="D32" t="n">
+        <v>343</v>
+      </c>
+      <c r="E32" t="n">
+        <v>12</v>
+      </c>
+      <c r="F32" t="n">
+        <v>65</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="n">
         <v>3</v>
-      </c>
-      <c r="E32" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" t="n">
-        <v>0</v>
-      </c>
-      <c r="G32" t="n">
-        <v>0</v>
-      </c>
-      <c r="H32" t="n">
-        <v>0</v>
       </c>
       <c r="I32" t="n">
         <v>0</v>
@@ -1568,12 +1568,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Penes</t>
+          <t>Pita</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>AB</t>
+          <t>-</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1582,19 +1582,19 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>343</v>
+        <v>250</v>
       </c>
       <c r="E33" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F33" t="n">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="G33" t="n">
         <v>0</v>
       </c>
       <c r="H33" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I33" t="n">
         <v>0</v>
@@ -1603,12 +1603,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Pita</t>
+          <t>Cheese</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Dirollo</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1617,33 +1617,33 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>250</v>
+        <v>272</v>
       </c>
       <c r="E34" t="n">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="F34" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H34" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="I34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Cheese</t>
+          <t>Tuna(water)</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Dirollo</t>
+          <t>AB</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1652,19 +1652,19 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>272</v>
+        <v>100</v>
       </c>
       <c r="E35" t="n">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F35" t="n">
         <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="H35" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="I35" t="n">
         <v>1</v>
@@ -1673,33 +1673,33 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Tuna(water)</t>
+          <t>Tortilla</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>AB</t>
+          <t>HighProtein</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>100g</t>
+          <t>1(62.5g)</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>100</v>
+        <v>197</v>
       </c>
       <c r="E36" t="n">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F36" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H36" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I36" t="n">
         <v>1</v>
@@ -1708,47 +1708,47 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Tortilla</t>
+          <t>Yogurt</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>HighProtein</t>
+          <t>Olympos</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>1(62.5g)</t>
+          <t>100g</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>197</v>
+        <v>72</v>
       </c>
       <c r="E37" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F37" t="n">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="G37" t="n">
+        <v>1</v>
+      </c>
+      <c r="H37" t="n">
         <v>2</v>
       </c>
-      <c r="H37" t="n">
-        <v>4</v>
-      </c>
       <c r="I37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Yogurt</t>
+          <t>Ground beef</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Olympos</t>
+          <t>Cooked(80-20)</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1757,19 +1757,19 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>72</v>
+        <v>246</v>
       </c>
       <c r="E38" t="n">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="F38" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H38" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="I38" t="n">
         <v>0</v>
@@ -1778,33 +1778,33 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Ground beef</t>
+          <t>Protein Powder</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Cooked(80-20)</t>
+          <t>Dymatize iso 100</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>100g</t>
+          <t>1 scoop (32g)</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>246</v>
+        <v>120</v>
       </c>
       <c r="E39" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F39" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G39" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H39" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="I39" t="n">
         <v>0</v>
@@ -1813,33 +1813,33 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Protein Powder</t>
+          <t>Granola</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Dymatize iso 100</t>
+          <t>Healthy Habits</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>1 scoop (32g)</t>
+          <t>100g</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>120</v>
+        <v>478</v>
       </c>
       <c r="E40" t="n">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F40" t="n">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="G40" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H40" t="n">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="I40" t="n">
         <v>0</v>
@@ -1848,33 +1848,33 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Granola</t>
+          <t>Almond Milk</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Healthy Habits</t>
+          <t>Olympos</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>100g</t>
+          <t>100ml</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>478</v>
+        <v>24</v>
       </c>
       <c r="E41" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F41" t="n">
-        <v>56</v>
+        <v>1</v>
       </c>
       <c r="G41" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H41" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="I41" t="n">
         <v>0</v>
@@ -1883,24 +1883,24 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Almond Milk</t>
+          <t>Egg whites</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Olympos</t>
+          <t>Xrysa Avga</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>100ml</t>
+          <t>100g</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="E42" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F42" t="n">
         <v>1</v>
@@ -1918,12 +1918,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Egg whites</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Xrysa Avga</t>
+          <t>Basmati (Indian)</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1932,19 +1932,19 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>46</v>
+        <v>358</v>
       </c>
       <c r="E43" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F43" t="n">
-        <v>1</v>
+        <v>78</v>
       </c>
       <c r="G43" t="n">
         <v>0</v>
       </c>
       <c r="H43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I43" t="n">
         <v>0</v>
@@ -1953,12 +1953,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Rice</t>
+          <t>Cashews</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Basmati (Indian)</t>
+          <t>EMMA</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1967,19 +1967,19 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>358</v>
+        <v>627</v>
       </c>
       <c r="E44" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F44" t="n">
-        <v>78</v>
+        <v>30</v>
       </c>
       <c r="G44" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H44" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="I44" t="n">
         <v>0</v>
@@ -1988,7 +1988,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Cashews</t>
+          <t>Walnuts</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2002,19 +2002,19 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>627</v>
+        <v>708</v>
       </c>
       <c r="E45" t="n">
         <v>17</v>
       </c>
       <c r="F45" t="n">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="G45" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H45" t="n">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="I45" t="n">
         <v>0</v>
@@ -2023,12 +2023,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Walnuts</t>
+          <t>Forest Fruits</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>EMMA</t>
+          <t>Gustona</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2037,19 +2037,19 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>708</v>
+        <v>43</v>
       </c>
       <c r="E46" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>5</v>
       </c>
       <c r="G46" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="H46" t="n">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="I46" t="n">
         <v>0</v>
@@ -2058,12 +2058,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Forest Fruits</t>
+          <t>PeanutButter</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Gustona</t>
+          <t>Haitoglou</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2072,33 +2072,33 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>43</v>
+        <v>610</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="F47" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="G47" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H47" t="n">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="I47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>PeanutButter</t>
+          <t>Dates</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Haitoglou</t>
+          <t>EMMA</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2107,33 +2107,33 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>610</v>
+        <v>469</v>
       </c>
       <c r="E48" t="n">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="F48" t="n">
-        <v>17</v>
+        <v>75</v>
       </c>
       <c r="G48" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H48" t="n">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="I48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Dates</t>
+          <t>Straberry Jam</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>EMMA</t>
+          <t>Health Habits</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2142,13 +2142,13 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>469</v>
+        <v>244</v>
       </c>
       <c r="E49" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="n">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="G49" t="n">
         <v>0</v>
@@ -2163,12 +2163,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Straberry Jam</t>
+          <t>yogurt</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Health Habits</t>
+          <t>Fage</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2177,19 +2177,19 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>244</v>
+        <v>70</v>
       </c>
       <c r="E50" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F50" t="n">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="G50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I50" t="n">
         <v>0</v>
@@ -2198,27 +2198,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>yogurt</t>
+          <t>Pita Kalampokiou</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Fage</t>
+          <t>Karamolegos</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>100g</t>
+          <t>1(82g)</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>70</v>
+        <v>217</v>
       </c>
       <c r="E51" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F51" t="n">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="G51" t="n">
         <v>1</v>
@@ -2227,53 +2227,53 @@
         <v>2</v>
       </c>
       <c r="I51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Pita Kalampokiou</t>
+          <t>Turkey Patties</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Karamolegos</t>
+          <t>Power in Meat</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>1(82g)</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>217</v>
+        <v>145</v>
       </c>
       <c r="E52" t="n">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="F52" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="G52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Turkey Patties</t>
+          <t>Rice Porridge</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Power in Meat</t>
+          <t>Gymbeam</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2282,13 +2282,13 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>145</v>
+        <v>348</v>
       </c>
       <c r="E53" t="n">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="F53" t="n">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="G53" t="n">
         <v>0</v>
@@ -2298,6 +2298,461 @@
       </c>
       <c r="I53" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>OliveOil</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>1 tablespoon</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>115</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" t="n">
+        <v>2</v>
+      </c>
+      <c r="H54" t="n">
+        <v>10</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Rice porridge - Speculus</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Prozis</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>100g</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>363</v>
+      </c>
+      <c r="E55" t="n">
+        <v>8</v>
+      </c>
+      <c r="F55" t="n">
+        <v>79</v>
+      </c>
+      <c r="G55" t="n">
+        <v>1</v>
+      </c>
+      <c r="H55" t="n">
+        <v>1</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chia </t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Alfa</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>100g</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>447</v>
+      </c>
+      <c r="E56" t="n">
+        <v>19</v>
+      </c>
+      <c r="F56" t="n">
+        <v>10</v>
+      </c>
+      <c r="G56" t="n">
+        <v>4</v>
+      </c>
+      <c r="H56" t="n">
+        <v>30</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Cacoa Powder</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Giotis</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>100g</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>360</v>
+      </c>
+      <c r="E57" t="n">
+        <v>20</v>
+      </c>
+      <c r="F57" t="n">
+        <v>9</v>
+      </c>
+      <c r="G57" t="n">
+        <v>13</v>
+      </c>
+      <c r="H57" t="n">
+        <v>21</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Protein Powder</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Prozis</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>100g</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>356</v>
+      </c>
+      <c r="E58" t="n">
+        <v>82</v>
+      </c>
+      <c r="F58" t="n">
+        <v>6</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" t="n">
+        <v>1</v>
+      </c>
+      <c r="I58" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Protein Shake</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>MyProtein</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>100g</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>399</v>
+      </c>
+      <c r="E59" t="n">
+        <v>61</v>
+      </c>
+      <c r="F59" t="n">
+        <v>15</v>
+      </c>
+      <c r="G59" t="n">
+        <v>2</v>
+      </c>
+      <c r="H59" t="n">
+        <v>6</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Milk 1.7%</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Olympos</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>100g</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>49</v>
+      </c>
+      <c r="E60" t="n">
+        <v>4</v>
+      </c>
+      <c r="F60" t="n">
+        <v>5</v>
+      </c>
+      <c r="G60" t="n">
+        <v>1</v>
+      </c>
+      <c r="H60" t="n">
+        <v>2</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Bueno</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Kinder</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>1(21.5g)</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>122</v>
+      </c>
+      <c r="E61" t="n">
+        <v>2</v>
+      </c>
+      <c r="F61" t="n">
+        <v>11</v>
+      </c>
+      <c r="G61" t="n">
+        <v>4</v>
+      </c>
+      <c r="H61" t="n">
+        <v>8</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Cottage</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Flair</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>100g</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>92</v>
+      </c>
+      <c r="E62" t="n">
+        <v>11</v>
+      </c>
+      <c r="F62" t="n">
+        <v>3</v>
+      </c>
+      <c r="G62" t="n">
+        <v>3</v>
+      </c>
+      <c r="H62" t="n">
+        <v>4</v>
+      </c>
+      <c r="I62" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Ygeias Almond</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Paulidis</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>100g</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>548</v>
+      </c>
+      <c r="E63" t="n">
+        <v>10</v>
+      </c>
+      <c r="F63" t="n">
+        <v>3</v>
+      </c>
+      <c r="G63" t="n">
+        <v>22</v>
+      </c>
+      <c r="H63" t="n">
+        <v>39</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Kefalotiri</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>AB</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>100g</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>350</v>
+      </c>
+      <c r="E64" t="n">
+        <v>27</v>
+      </c>
+      <c r="F64" t="n">
+        <v>1</v>
+      </c>
+      <c r="G64" t="n">
+        <v>17</v>
+      </c>
+      <c r="H64" t="n">
+        <v>27</v>
+      </c>
+      <c r="I64" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Pennes_Olikis</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Melissa</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>100g</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>355</v>
+      </c>
+      <c r="E65" t="n">
+        <v>13</v>
+      </c>
+      <c r="F65" t="n">
+        <v>68</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0</v>
+      </c>
+      <c r="H65" t="n">
+        <v>2</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Pesto</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Barilla</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>100g</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>482</v>
+      </c>
+      <c r="E66" t="n">
+        <v>5</v>
+      </c>
+      <c r="F66" t="n">
+        <v>10</v>
+      </c>
+      <c r="G66" t="n">
+        <v>5</v>
+      </c>
+      <c r="H66" t="n">
+        <v>46</v>
+      </c>
+      <c r="I66" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>